<commit_message>
Prosthetic Didgets (Continued) 업데이트
#831
</commit_message>
<xml_diff>
--- a/Data/Mlie/Prosthetic Didgets (Continued) - 2012507402/2012507402.xlsx
+++ b/Data/Mlie/Prosthetic Didgets (Continued) - 2012507402/2012507402.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.11\Prosthetic Didgets (Continued) - 2012507402\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Mlie\Prosthetic Didgets (Continued) - 2012507402\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1523D9-5AB6-49E9-9720-926CC18DB6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B57D62-0257-4881-977C-1F953ADD6734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240414" sheetId="1" r:id="rId1"/>
-    <sheet name="Merge_RKTM" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_240511" sheetId="4" r:id="rId1"/>
+    <sheet name="240414" sheetId="1" r:id="rId2"/>
+    <sheet name="Merge_RKTM" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="178">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -525,6 +526,51 @@
   <si>
     <t>이식 수술 중</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>막대기같은 발가락 모형으로 걷는것을 좀더 편하게 만들어줍니다.</t>
+  </si>
+  <si>
+    <t>단순한 발가락 모형</t>
+  </si>
+  <si>
+    <t>막대기같은 손가락 모형으로 쥐는 행동을 좀더 편하게 만들어줍니다.</t>
+  </si>
+  <si>
+    <t>단순한 손가락 모형</t>
+  </si>
+  <si>
+    <t>이식 수술 중</t>
+  </si>
+  <si>
+    <t>단순한 발가락 모형을 이식합니다.</t>
+  </si>
+  <si>
+    <t>단순한 발가락 모형 이식</t>
+  </si>
+  <si>
+    <t>단순한 손가락 모형을 이식합니다.</t>
+  </si>
+  <si>
+    <t>단순한 손가락 모형 이식</t>
+  </si>
+  <si>
+    <t>이식된 생체공학 발가락.</t>
+  </si>
+  <si>
+    <t>이식된 생체공학 손가락.</t>
+  </si>
+  <si>
+    <t>이식된 간단한 인공 발가락.</t>
+  </si>
+  <si>
+    <t>이식된 간단한 인공 손가락.</t>
+  </si>
+  <si>
+    <t>이식된 단순한 발가락 모형.</t>
+  </si>
+  <si>
+    <t>이식된 단순한 손가락 모형.</t>
   </si>
 </sst>
 </file>
@@ -909,10 +955,769 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7682B-E543-4F1F-9116-D492D98D2784}">
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="44.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="68.6328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1836,7 +2641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299B55C6-1F07-45E0-B301-C1FBEBCE2083}">
   <dimension ref="A2:E37"/>
   <sheetViews>
@@ -1863,7 +2668,7 @@
         <v>119</v>
       </c>
       <c r="E2">
-        <f>IF(ISERROR(B2),"",MATCH(C2,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B2),"",MATCH(C2,'240414'!$A$2:$A$43,0))</f>
         <v>9</v>
       </c>
     </row>
@@ -1879,7 +2684,7 @@
         <v>120</v>
       </c>
       <c r="E3">
-        <f>IF(ISERROR(B3),"",MATCH(C3,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B3),"",MATCH(C3,'240414'!$A$2:$A$43,0))</f>
         <v>11</v>
       </c>
     </row>
@@ -1895,7 +2700,7 @@
         <v>121</v>
       </c>
       <c r="E4">
-        <f>IF(ISERROR(B4),"",MATCH(C4,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B4),"",MATCH(C4,'240414'!$A$2:$A$43,0))</f>
         <v>5</v>
       </c>
     </row>
@@ -1911,7 +2716,7 @@
         <v>122</v>
       </c>
       <c r="E5">
-        <f>IF(ISERROR(B5),"",MATCH(C5,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B5),"",MATCH(C5,'240414'!$A$2:$A$43,0))</f>
         <v>7</v>
       </c>
     </row>
@@ -1927,7 +2732,7 @@
         <v>123</v>
       </c>
       <c r="E6">
-        <f>IF(ISERROR(B6),"",MATCH(C6,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B6),"",MATCH(C6,'240414'!$A$2:$A$43,0))</f>
         <v>26</v>
       </c>
     </row>
@@ -1943,7 +2748,7 @@
         <v>124</v>
       </c>
       <c r="E7">
-        <f>IF(ISERROR(B7),"",MATCH(C7,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B7),"",MATCH(C7,'240414'!$A$2:$A$43,0))</f>
         <v>27</v>
       </c>
     </row>
@@ -1959,7 +2764,7 @@
         <v>125</v>
       </c>
       <c r="E8">
-        <f>IF(ISERROR(B8),"",MATCH(C8,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B8),"",MATCH(C8,'240414'!$A$2:$A$43,0))</f>
         <v>25</v>
       </c>
     </row>
@@ -1975,7 +2780,7 @@
         <v>126</v>
       </c>
       <c r="E9">
-        <f>IF(ISERROR(B9),"",MATCH(C9,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B9),"",MATCH(C9,'240414'!$A$2:$A$43,0))</f>
         <v>29</v>
       </c>
     </row>
@@ -1991,7 +2796,7 @@
         <v>124</v>
       </c>
       <c r="E10">
-        <f>IF(ISERROR(B10),"",MATCH(C10,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B10),"",MATCH(C10,'240414'!$A$2:$A$43,0))</f>
         <v>30</v>
       </c>
     </row>
@@ -2007,7 +2812,7 @@
         <v>127</v>
       </c>
       <c r="E11">
-        <f>IF(ISERROR(B11),"",MATCH(C11,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B11),"",MATCH(C11,'240414'!$A$2:$A$43,0))</f>
         <v>28</v>
       </c>
     </row>
@@ -2023,7 +2828,7 @@
         <v>128</v>
       </c>
       <c r="E12">
-        <f>IF(ISERROR(B12),"",MATCH(C12,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B12),"",MATCH(C12,'240414'!$A$2:$A$43,0))</f>
         <v>20</v>
       </c>
     </row>
@@ -2039,7 +2844,7 @@
         <v>124</v>
       </c>
       <c r="E13">
-        <f>IF(ISERROR(B13),"",MATCH(C13,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B13),"",MATCH(C13,'240414'!$A$2:$A$43,0))</f>
         <v>21</v>
       </c>
     </row>
@@ -2055,7 +2860,7 @@
         <v>129</v>
       </c>
       <c r="E14">
-        <f>IF(ISERROR(B14),"",MATCH(C14,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B14),"",MATCH(C14,'240414'!$A$2:$A$43,0))</f>
         <v>19</v>
       </c>
     </row>
@@ -2071,7 +2876,7 @@
         <v>130</v>
       </c>
       <c r="E15">
-        <f>IF(ISERROR(B15),"",MATCH(C15,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B15),"",MATCH(C15,'240414'!$A$2:$A$43,0))</f>
         <v>23</v>
       </c>
     </row>
@@ -2087,7 +2892,7 @@
         <v>124</v>
       </c>
       <c r="E16">
-        <f>IF(ISERROR(B16),"",MATCH(C16,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B16),"",MATCH(C16,'240414'!$A$2:$A$43,0))</f>
         <v>24</v>
       </c>
     </row>
@@ -2103,7 +2908,7 @@
         <v>131</v>
       </c>
       <c r="E17">
-        <f>IF(ISERROR(B17),"",MATCH(C17,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B17),"",MATCH(C17,'240414'!$A$2:$A$43,0))</f>
         <v>22</v>
       </c>
     </row>
@@ -2123,7 +2928,7 @@
         <v>133</v>
       </c>
       <c r="E18" t="str">
-        <f>IF(ISERROR(B18),"",MATCH(C18,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B18),"",MATCH(C18,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2143,7 +2948,7 @@
         <v>135</v>
       </c>
       <c r="E19" t="str">
-        <f>IF(ISERROR(B19),"",MATCH(C19,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B19),"",MATCH(C19,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2163,7 +2968,7 @@
         <v>137</v>
       </c>
       <c r="E20" t="str">
-        <f>IF(ISERROR(B20),"",MATCH(C20,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B20),"",MATCH(C20,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2183,7 +2988,7 @@
         <v>139</v>
       </c>
       <c r="E21" t="str">
-        <f>IF(ISERROR(B21),"",MATCH(C21,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B21),"",MATCH(C21,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2203,7 +3008,7 @@
         <v>141</v>
       </c>
       <c r="E22" t="str">
-        <f>IF(ISERROR(B22),"",MATCH(C22,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B22),"",MATCH(C22,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2223,7 +3028,7 @@
         <v>143</v>
       </c>
       <c r="E23" t="str">
-        <f>IF(ISERROR(B23),"",MATCH(C23,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B23),"",MATCH(C23,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2243,7 +3048,7 @@
         <v>145</v>
       </c>
       <c r="E24" t="str">
-        <f>IF(ISERROR(B24),"",MATCH(C24,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B24),"",MATCH(C24,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2263,7 +3068,7 @@
         <v>147</v>
       </c>
       <c r="E25" t="str">
-        <f>IF(ISERROR(B25),"",MATCH(C25,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B25),"",MATCH(C25,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2283,7 +3088,7 @@
         <v>149</v>
       </c>
       <c r="E26" t="str">
-        <f>IF(ISERROR(B26),"",MATCH(C26,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B26),"",MATCH(C26,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2303,7 +3108,7 @@
         <v>151</v>
       </c>
       <c r="E27" t="str">
-        <f>IF(ISERROR(B27),"",MATCH(C27,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B27),"",MATCH(C27,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2323,7 +3128,7 @@
         <v>153</v>
       </c>
       <c r="E28" t="str">
-        <f>IF(ISERROR(B28),"",MATCH(C28,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B28),"",MATCH(C28,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2343,7 +3148,7 @@
         <v>155</v>
       </c>
       <c r="E29" t="str">
-        <f>IF(ISERROR(B29),"",MATCH(C29,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B29),"",MATCH(C29,'240414'!$A$2:$A$43,0))</f>
         <v/>
       </c>
     </row>
@@ -2359,7 +3164,7 @@
         <v>156</v>
       </c>
       <c r="E30">
-        <f>IF(ISERROR(B30),"",MATCH(C30,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B30),"",MATCH(C30,'240414'!$A$2:$A$43,0))</f>
         <v>40</v>
       </c>
     </row>
@@ -2375,7 +3180,7 @@
         <v>119</v>
       </c>
       <c r="E31">
-        <f>IF(ISERROR(B31),"",MATCH(C31,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B31),"",MATCH(C31,'240414'!$A$2:$A$43,0))</f>
         <v>39</v>
       </c>
     </row>
@@ -2391,7 +3196,7 @@
         <v>157</v>
       </c>
       <c r="E32">
-        <f>IF(ISERROR(B32),"",MATCH(C32,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B32),"",MATCH(C32,'240414'!$A$2:$A$43,0))</f>
         <v>42</v>
       </c>
     </row>
@@ -2407,7 +3212,7 @@
         <v>120</v>
       </c>
       <c r="E33">
-        <f>IF(ISERROR(B33),"",MATCH(C33,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B33),"",MATCH(C33,'240414'!$A$2:$A$43,0))</f>
         <v>41</v>
       </c>
     </row>
@@ -2423,7 +3228,7 @@
         <v>158</v>
       </c>
       <c r="E34">
-        <f>IF(ISERROR(B34),"",MATCH(C34,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B34),"",MATCH(C34,'240414'!$A$2:$A$43,0))</f>
         <v>36</v>
       </c>
     </row>
@@ -2439,7 +3244,7 @@
         <v>121</v>
       </c>
       <c r="E35">
-        <f>IF(ISERROR(B35),"",MATCH(C35,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B35),"",MATCH(C35,'240414'!$A$2:$A$43,0))</f>
         <v>35</v>
       </c>
     </row>
@@ -2455,7 +3260,7 @@
         <v>159</v>
       </c>
       <c r="E36">
-        <f>IF(ISERROR(B36),"",MATCH(C36,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B36),"",MATCH(C36,'240414'!$A$2:$A$43,0))</f>
         <v>38</v>
       </c>
     </row>
@@ -2471,7 +3276,7 @@
         <v>122</v>
       </c>
       <c r="E37">
-        <f>IF(ISERROR(B37),"",MATCH(C37,Main_240414!$A$2:$A$43,0))</f>
+        <f>IF(ISERROR(B37),"",MATCH(C37,'240414'!$A$2:$A$43,0))</f>
         <v>37</v>
       </c>
     </row>

</xml_diff>